<commit_message>
TORIBDA feat: added loadAllItemsInfo method
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B4A4B-B4BA-466B-AD03-2B9FF2089CF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A078FE0-C569-4367-8228-B07797830DA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Plan</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>30mins</t>
+  </si>
+  <si>
+    <t>2 mins</t>
+  </si>
+  <si>
+    <t>1 min 47 seconds</t>
+  </si>
+  <si>
+    <t>have just used the static method from ItemDataLoader</t>
+  </si>
+  <si>
+    <t>I may use the public static methods from ItemDataLoader, which could make tasks easier</t>
   </si>
   <si>
     <t>I can try to do pseudocodes at first rather than try to code instantly</t>
@@ -456,7 +468,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E8"/>
+      <selection activeCell="B4" sqref="B4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,18 +506,30 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TORIBDA feat: added calculateReceipt method and Receipt Class
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A078FE0-C569-4367-8228-B07797830DA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EE3041-A6F7-4888-BF50-9C56182DF3D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Plan</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>I can try to do pseudocodes at first rather than try to code instantly</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>9 mins 43 seconds</t>
+  </si>
+  <si>
+    <t>have only created pseudocode and added method names for the sub-tasks</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>1hr 27mins</t>
@@ -468,7 +480,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E8"/>
+      <selection activeCell="B5" sqref="B5:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,10 +518,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
@@ -532,9 +544,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TORIBDA feat: added calculateItemSubtotal
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EE3041-A6F7-4888-BF50-9C56182DF3D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF05DB3-A15C-47AC-9ADB-0EA05DCE3956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Plan</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>have only created pseudocode and added method names for the sub-tasks</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
+  <si>
+    <t>2 mins 37 seconds</t>
   </si>
   <si>
     <t>-</t>
@@ -480,7 +486,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E8"/>
+      <selection activeCell="B6" sqref="B6:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +524,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
@@ -558,12 +564,24 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TORIBDA feat: added calculateTotalPrice method
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF05DB3-A15C-47AC-9ADB-0EA05DCE3956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF932BF-C694-435A-8AF8-194E3534F613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Plan</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>2 mins 37 seconds</t>
+  </si>
+  <si>
+    <t>1 min 28 seconds</t>
   </si>
   <si>
     <t>-</t>
@@ -486,7 +489,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E8"/>
+      <selection activeCell="B7" sqref="B7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,10 +527,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
@@ -564,7 +567,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,15 +581,27 @@
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TORIBDA feat: added generateReceipt method
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF932BF-C694-435A-8AF8-194E3534F613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B641D4-6530-46F7-B55D-0AF4E5E2FD94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Plan</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Time spent more on identifying on how to approach the convertion from barcodes into an item class while utilizing the existing classes.</t>
+  </si>
+  <si>
+    <t>7 mins 18 seconds</t>
+  </si>
+  <si>
+    <t>have only created pseudocode and added the method for the sub-tasks all the while setting the receipt format</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E8"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,9 +610,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TORIBDA feat: added generateItemsDetail method
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitvob\posMachinePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B641D4-6530-46F7-B55D-0AF4E5E2FD94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45F1A90-E389-4A64-8B4B-3599456582CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12210" yWindow="2625" windowWidth="16230" windowHeight="12960" xr2:uid="{D3D3D164-0338-412A-B605-2187C02C5DDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Plan</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Time spent more on identifying on how to approach the convertion from barcodes into an item class while utilizing the existing classes.</t>
+  </si>
+  <si>
+    <t>3 mins</t>
+  </si>
+  <si>
+    <t>12 mins 27 seconds</t>
+  </si>
+  <si>
+    <t>Time spent more on formatting so that the PosMachineTest would result to success</t>
+  </si>
+  <si>
+    <t>Check the required formatting rather than code blindly of whatever format (try not to overlook when there is a provided format).</t>
   </si>
   <si>
     <t>7 mins 18 seconds</t>
@@ -495,7 +507,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,18 +630,30 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>